<commit_message>
unit test millimeter accuracy, fixed bug where width/height was integer always
</commit_message>
<xml_diff>
--- a/tests/test_paklijsten/paklijst4.xlsx
+++ b/tests/test_paklijsten/paklijst4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\HDS\2d_rectangle_packing\tests\test_paklijsten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E063A9-FCF7-443A-ACBE-573B0FE0AE75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33CECDF-CA44-4DF7-A330-99BD99ABAAA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7296" yWindow="3084" windowWidth="17280" windowHeight="8964" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paklijst_zonder_opmaak" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="116">
   <si>
     <t>Aantal</t>
   </si>
@@ -455,6 +455,24 @@
   </si>
   <si>
     <t>Batch/Coupage</t>
+  </si>
+  <si>
+    <t>50,1</t>
+  </si>
+  <si>
+    <t>80,5</t>
+  </si>
+  <si>
+    <t>50,2</t>
+  </si>
+  <si>
+    <t>80,2</t>
+  </si>
+  <si>
+    <t>44,8</t>
+  </si>
+  <si>
+    <t>74,1</t>
   </si>
 </sst>
 </file>
@@ -921,7 +939,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,11 +1002,11 @@
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2">
-        <v>50.1</v>
-      </c>
-      <c r="E2">
-        <v>80.5</v>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>111</v>
       </c>
       <c r="F2">
         <v>44176</v>
@@ -1019,11 +1037,11 @@
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3">
-        <v>50.2</v>
-      </c>
-      <c r="E3">
-        <v>80.2</v>
+      <c r="D3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" t="s">
+        <v>113</v>
       </c>
       <c r="F3">
         <v>44176</v>
@@ -1054,11 +1072,11 @@
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4">
-        <v>44.8</v>
-      </c>
-      <c r="E4">
-        <v>74.099999999999994</v>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" t="s">
+        <v>115</v>
       </c>
       <c r="F4">
         <v>44146</v>

</xml_diff>

<commit_message>
fixed bug of stacking smaller grid widths in larger but code is not really clean --> needs refactoring
</commit_message>
<xml_diff>
--- a/tests/test_paklijsten/paklijst4.xlsx
+++ b/tests/test_paklijsten/paklijst4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\HDS\2d_rectangle_packing\tests\test_paklijsten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6359B8FC-176F-4833-8EF2-5449606B941C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E393EE55-A37A-4D76-898C-3645881DE496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paklijst_zonder_opmaak" sheetId="1" r:id="rId1"/>
@@ -948,7 +948,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>